<commit_message>
removed unnecessary file formatting, added proportion choice to analyzeEffort.m
</commit_message>
<xml_diff>
--- a/data/monetary/M_3101.xlsx
+++ b/data/monetary/M_3101.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11114"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tun46412\Documents\GitHub\istart\Mock_Scan\Monetary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jameswyngaarden/Documents/GitHub/istart-effort/data/monetary/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37E2B97A-DF84-FC41-84EE-8DA6B74740F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4190"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="17100" windowHeight="9000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="M_3101" sheetId="1" r:id="rId1"/>
@@ -174,7 +175,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -977,16 +978,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1099,7 +1100,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -1182,7 +1183,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -1265,7 +1266,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -1348,7 +1349,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>37</v>
       </c>
@@ -1431,7 +1432,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>37</v>
       </c>
@@ -1535,7 +1536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>37</v>
       </c>
@@ -1639,7 +1640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -1743,7 +1744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>37</v>
       </c>
@@ -1847,7 +1848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>37</v>
       </c>
@@ -1951,7 +1952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>37</v>
       </c>
@@ -2055,7 +2056,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>37</v>
       </c>
@@ -2159,7 +2160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>37</v>
       </c>
@@ -2263,7 +2264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>37</v>
       </c>
@@ -2367,7 +2368,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>37</v>
       </c>
@@ -2471,7 +2472,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>37</v>
       </c>
@@ -2575,7 +2576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>37</v>
       </c>
@@ -2679,7 +2680,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>37</v>
       </c>
@@ -2783,7 +2784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>37</v>
       </c>
@@ -2887,7 +2888,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -2991,7 +2992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>37</v>
       </c>
@@ -3095,7 +3096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>37</v>
       </c>
@@ -3199,7 +3200,7 @@
         <v>3.58</v>
       </c>
     </row>
-    <row r="23" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>37</v>
       </c>
@@ -3303,7 +3304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>37</v>
       </c>
@@ -3407,7 +3408,7 @@
         <v>4.12</v>
       </c>
     </row>
-    <row r="25" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>37</v>
       </c>
@@ -3511,7 +3512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>37</v>
       </c>
@@ -3615,7 +3616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>37</v>
       </c>
@@ -3719,7 +3720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>37</v>
       </c>
@@ -3823,7 +3824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>37</v>
       </c>
@@ -3927,7 +3928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>37</v>
       </c>
@@ -4031,7 +4032,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>37</v>
       </c>
@@ -4135,7 +4136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>37</v>
       </c>
@@ -4239,7 +4240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>37</v>
       </c>
@@ -4343,7 +4344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>37</v>
       </c>
@@ -4447,7 +4448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>37</v>
       </c>
@@ -4551,7 +4552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>37</v>
       </c>
@@ -4655,7 +4656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>37</v>
       </c>
@@ -4759,7 +4760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -4863,7 +4864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -4967,7 +4968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>37</v>
       </c>
@@ -5071,7 +5072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>37</v>
       </c>
@@ -5175,7 +5176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>37</v>
       </c>
@@ -5279,7 +5280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>37</v>
       </c>
@@ -5383,7 +5384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>37</v>
       </c>
@@ -5487,7 +5488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>37</v>
       </c>
@@ -5591,7 +5592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>37</v>
       </c>
@@ -5695,7 +5696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>37</v>
       </c>
@@ -5799,7 +5800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>37</v>
       </c>
@@ -5903,7 +5904,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>37</v>
       </c>
@@ -6007,7 +6008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>37</v>
       </c>
@@ -6111,7 +6112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>37</v>
       </c>
@@ -6215,7 +6216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>37</v>
       </c>
@@ -6319,7 +6320,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>37</v>
       </c>
@@ -6423,7 +6424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>37</v>
       </c>
@@ -6527,7 +6528,7 @@
         <v>3.94</v>
       </c>
     </row>
-    <row r="55" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>37</v>
       </c>
@@ -6631,7 +6632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>37</v>
       </c>
@@ -6735,7 +6736,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>37</v>
       </c>

</xml_diff>